<commit_message>
Add function to convert 'drop view' and some of test cases in 2020.05.03
</commit_message>
<xml_diff>
--- a/test/PlSql2PostgreTestCase.xlsx
+++ b/test/PlSql2PostgreTestCase.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="359">
   <si>
     <t>項番</t>
     <rPh sb="0" eb="1">
@@ -1754,47 +1754,107 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t xml:space="preserve">CREATE PUBLIC SYNONYM TEST_SYM FOR TEST_TBL;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CREATE SYNONYM TEST_USER.TEST_SYM FOR TEST_USER.TEST_TBL;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CREATE VIEW TEST_USER.TEST_SYM AS SELECT * FROM TEST_USER.TEST_TBL;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">create synonym test_sym for test_tbl;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">create public synonym test_sym for test_tbl;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">create VIEW test_sym AS SELECT * FROM test_tbl;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">create synonym test_user.test_sym for test_user.test_tbl;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">create VIEW test_user.test_sym AS SELECT * FROM test_user.test_tbl;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CREATE  VIEW TEST_SYM AS SELECT * FROM TEST_TBL;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>削除</t>
+    <rPh sb="0" eb="2">
+      <t>サクジョ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>最小要素</t>
+    <rPh sb="0" eb="2">
+      <t>サイショウ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ヨウソ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>小文字</t>
+    <rPh sb="0" eb="3">
+      <t>コモジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>大文字</t>
+    <rPh sb="0" eb="3">
+      <t>オオモジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PUBLICオブジェクト</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">drop synonym test_sym;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">DROP SYNONYM TEST_SYM;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">drop VIEW test_sym;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t xml:space="preserve">CREATE VIEW TEST_SYM AS SELECT * FROM TEST_TBL;
 </t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">CREATE PUBLIC SYNONYM TEST_SYM FOR TEST_TBL;
-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CREATE SYNONYM TEST_USER.TEST_SYM FOR TEST_USER.TEST_TBL;
-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CREATE VIEW TEST_USER.TEST_SYM AS SELECT * FROM TEST_USER.TEST_TBL;
-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">create synonym test_sym for test_tbl;
-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">create public synonym test_sym for test_tbl;
-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">create VIEW test_sym AS SELECT * FROM test_tbl;
-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">create synonym test_user.test_sym for test_user.test_tbl;
-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">create VIEW test_user.test_sym AS SELECT * FROM test_user.test_tbl;
+    <t xml:space="preserve">DROP VIEW TEST_SYM;
 </t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1804,7 +1864,142 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">CREATE  VIEW TEST_SYM AS SELECT * FROM TEST_TBL;
+    <t xml:space="preserve">drop public synonym test_sym;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">drop  VIEW test_sym;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">DROP PUBLIC SYNONYM TEST_SYM;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">DROP  VIEW TEST_SYM;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スキーマ付き</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">drop synonym test_user.test_sym;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">DROP SYNONYM TEST_USER.TEST_SYM;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">DROP VIEW TEST_USER.TEST_SYM;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">drop VIEW test_user.test_sym;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>強制削除</t>
+    <rPh sb="0" eb="2">
+      <t>キョウセイ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>サクジョ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">drop synonym test_sym force;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">DROP SYNONYM TEST_SYM FORCE;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">drop VIEW test_sym CASCADE;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">DROP VIEW TEST_SYM CASCADE;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>強制削除</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>シノニム</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>シノニム</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ビュー</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">drop view test_sym;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">DROP VIEW TEST_SYM;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">drop view test_user.test_sym;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">drop view test_sym CASCADE;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">drop view test_user.test_sym CASCADE;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">DROP VIEW TEST_USER.TEST_SYM CASCADE;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">drop view test_sym cascade constraints;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">DROP VIEW TEST_SYM CASCADE CONSTRAINTS;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">drop view test_sym cascade ;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">DROP VIEW TEST_SYM CASCADE ;
 </t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1813,7 +2008,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1848,6 +2043,12 @@
       <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1923,7 +2124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1942,6 +2143,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -2246,13 +2449,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G124"/>
+  <dimension ref="A1:G138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G117" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G129" sqref="G129"/>
+    <sheetView tabSelected="1" topLeftCell="A123" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F125" sqref="F125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="5.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.25" bestFit="1" customWidth="1"/>
@@ -2270,7 +2473,7 @@
     <col min="15" max="15" width="15.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2293,7 +2496,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <f t="shared" ref="A2:A121" si="0">ROW()-1</f>
         <v>1</v>
@@ -2317,7 +2520,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="27">
+    <row r="3" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -2341,7 +2544,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="27">
+    <row r="4" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <f>ROW()-1</f>
         <v>3</v>
@@ -2365,7 +2568,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="27">
+    <row r="5" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <f t="shared" ref="A5:A68" si="1">ROW()-1</f>
         <v>4</v>
@@ -2389,7 +2592,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="27">
+    <row r="6" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -2413,7 +2616,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="27">
+    <row r="7" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -2437,7 +2640,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="27">
+    <row r="8" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -2461,7 +2664,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="27">
+    <row r="9" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -2485,7 +2688,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="27">
+    <row r="10" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -2509,7 +2712,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="27">
+    <row r="11" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -2533,7 +2736,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="27">
+    <row r="12" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A12" s="2">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -2557,7 +2760,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="27">
+    <row r="13" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -2581,7 +2784,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="27">
+    <row r="14" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A14" s="2">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -2605,7 +2808,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="27">
+    <row r="15" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A15" s="2">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -2629,7 +2832,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="27">
+    <row r="16" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A16" s="2">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -2653,7 +2856,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="27">
+    <row r="17" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A17" s="2">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -2677,7 +2880,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="27">
+    <row r="18" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A18" s="2">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -2701,7 +2904,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="27">
+    <row r="19" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A19" s="2">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -2725,7 +2928,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="27">
+    <row r="20" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A20" s="2">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -2749,7 +2952,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="27">
+    <row r="21" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A21" s="2">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -2773,7 +2976,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="27">
+    <row r="22" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A22" s="2">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -2797,7 +3000,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="27">
+    <row r="23" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A23" s="2">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -2821,7 +3024,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="27">
+    <row r="24" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A24" s="2">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -2845,7 +3048,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="27">
+    <row r="25" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A25" s="2">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -2869,7 +3072,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="27">
+    <row r="26" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A26" s="2">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -2893,7 +3096,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="27">
+    <row r="27" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A27" s="2">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -2917,7 +3120,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="27">
+    <row r="28" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A28" s="2">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -2941,7 +3144,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="27">
+    <row r="29" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A29" s="2">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -2965,7 +3168,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="27">
+    <row r="30" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A30" s="2">
         <f t="shared" si="1"/>
         <v>29</v>
@@ -2989,7 +3192,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="27">
+    <row r="31" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A31" s="2">
         <f t="shared" si="1"/>
         <v>30</v>
@@ -3013,7 +3216,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="27">
+    <row r="32" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A32" s="2">
         <f t="shared" si="1"/>
         <v>31</v>
@@ -3037,7 +3240,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="40.5">
+    <row r="33" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A33" s="2">
         <f t="shared" si="1"/>
         <v>32</v>
@@ -3061,7 +3264,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="40.5">
+    <row r="34" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A34" s="2">
         <f t="shared" si="1"/>
         <v>33</v>
@@ -3085,7 +3288,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="40.5">
+    <row r="35" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A35" s="2">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -3109,7 +3312,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="40.5">
+    <row r="36" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A36" s="2">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -3133,7 +3336,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="40.5">
+    <row r="37" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A37" s="2">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -3157,7 +3360,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="40.5">
+    <row r="38" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A38" s="2">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -3181,7 +3384,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="40.5">
+    <row r="39" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A39" s="2">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -3205,7 +3408,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="27">
+    <row r="40" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A40" s="2">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -3229,7 +3432,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="27">
+    <row r="41" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A41" s="2">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -3253,7 +3456,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="27">
+    <row r="42" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A42" s="2">
         <f t="shared" si="1"/>
         <v>41</v>
@@ -3277,7 +3480,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="27">
+    <row r="43" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A43" s="2">
         <f t="shared" si="1"/>
         <v>42</v>
@@ -3301,7 +3504,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="27">
+    <row r="44" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A44" s="2">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -3325,7 +3528,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="27">
+    <row r="45" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A45" s="2">
         <f t="shared" si="1"/>
         <v>44</v>
@@ -3349,7 +3552,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="27">
+    <row r="46" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A46" s="2">
         <f t="shared" si="1"/>
         <v>45</v>
@@ -3373,7 +3576,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="27">
+    <row r="47" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A47" s="2">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -3397,7 +3600,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="27">
+    <row r="48" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A48" s="2">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -3421,7 +3624,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="27">
+    <row r="49" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A49" s="2">
         <f t="shared" si="1"/>
         <v>48</v>
@@ -3445,7 +3648,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="27">
+    <row r="50" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A50" s="2">
         <f t="shared" si="1"/>
         <v>49</v>
@@ -3469,7 +3672,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="27">
+    <row r="51" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A51" s="2">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -3493,7 +3696,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="27">
+    <row r="52" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A52" s="2">
         <f t="shared" si="1"/>
         <v>51</v>
@@ -3517,7 +3720,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="40.5">
+    <row r="53" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A53" s="2">
         <f t="shared" si="1"/>
         <v>52</v>
@@ -3541,7 +3744,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="40.5">
+    <row r="54" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A54" s="2">
         <f t="shared" si="1"/>
         <v>53</v>
@@ -3565,7 +3768,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="40.5">
+    <row r="55" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A55" s="2">
         <f t="shared" si="1"/>
         <v>54</v>
@@ -3589,7 +3792,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="40.5">
+    <row r="56" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A56" s="2">
         <f t="shared" si="1"/>
         <v>55</v>
@@ -3613,7 +3816,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="40.5">
+    <row r="57" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A57" s="2">
         <f t="shared" si="1"/>
         <v>56</v>
@@ -3637,7 +3840,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="40.5">
+    <row r="58" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A58" s="2">
         <f t="shared" si="1"/>
         <v>57</v>
@@ -3661,7 +3864,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="40.5">
+    <row r="59" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A59" s="2">
         <f t="shared" si="1"/>
         <v>58</v>
@@ -3685,7 +3888,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="40.5">
+    <row r="60" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A60" s="2">
         <f t="shared" si="1"/>
         <v>59</v>
@@ -3709,7 +3912,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="40.5">
+    <row r="61" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A61" s="2">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -3733,7 +3936,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="40.5">
+    <row r="62" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A62" s="2">
         <f t="shared" si="1"/>
         <v>61</v>
@@ -3757,7 +3960,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="40.5">
+    <row r="63" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A63" s="2">
         <f t="shared" si="1"/>
         <v>62</v>
@@ -3781,7 +3984,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="40.5">
+    <row r="64" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A64" s="2">
         <f t="shared" si="1"/>
         <v>63</v>
@@ -3805,7 +4008,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="40.5">
+    <row r="65" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A65" s="2">
         <f t="shared" si="1"/>
         <v>64</v>
@@ -3829,7 +4032,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="40.5">
+    <row r="66" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A66" s="2">
         <f t="shared" si="1"/>
         <v>65</v>
@@ -3853,7 +4056,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="40.5">
+    <row r="67" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A67" s="2">
         <f t="shared" si="1"/>
         <v>66</v>
@@ -3877,7 +4080,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="40.5">
+    <row r="68" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A68" s="2">
         <f t="shared" si="1"/>
         <v>67</v>
@@ -3901,7 +4104,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="40.5">
+    <row r="69" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A69" s="2">
         <f t="shared" si="0"/>
         <v>68</v>
@@ -3925,7 +4128,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="40.5">
+    <row r="70" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A70" s="2">
         <f t="shared" si="0"/>
         <v>69</v>
@@ -3949,7 +4152,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="40.5">
+    <row r="71" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A71" s="2">
         <f t="shared" si="0"/>
         <v>70</v>
@@ -3973,7 +4176,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="40.5">
+    <row r="72" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A72" s="2">
         <f t="shared" si="0"/>
         <v>71</v>
@@ -3997,7 +4200,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="40.5">
+    <row r="73" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A73" s="2">
         <f t="shared" si="0"/>
         <v>72</v>
@@ -4021,7 +4224,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="40.5">
+    <row r="74" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A74" s="2">
         <f t="shared" si="0"/>
         <v>73</v>
@@ -4045,7 +4248,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="40.5">
+    <row r="75" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A75" s="2">
         <f t="shared" si="0"/>
         <v>74</v>
@@ -4069,7 +4272,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="40.5">
+    <row r="76" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A76" s="2">
         <f t="shared" si="0"/>
         <v>75</v>
@@ -4093,7 +4296,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="27">
+    <row r="77" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A77" s="2">
         <f t="shared" si="0"/>
         <v>76</v>
@@ -4117,7 +4320,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="27">
+    <row r="78" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A78" s="2">
         <f t="shared" si="0"/>
         <v>77</v>
@@ -4141,7 +4344,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="27">
+    <row r="79" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A79" s="2">
         <f t="shared" si="0"/>
         <v>78</v>
@@ -4165,7 +4368,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="27">
+    <row r="80" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A80" s="2">
         <f t="shared" si="0"/>
         <v>79</v>
@@ -4189,7 +4392,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="27">
+    <row r="81" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A81" s="2">
         <f t="shared" si="0"/>
         <v>80</v>
@@ -4213,7 +4416,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="27">
+    <row r="82" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A82" s="2">
         <f t="shared" si="0"/>
         <v>81</v>
@@ -4237,7 +4440,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="27">
+    <row r="83" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A83" s="2">
         <f t="shared" si="0"/>
         <v>82</v>
@@ -4261,7 +4464,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="27">
+    <row r="84" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A84" s="2">
         <f t="shared" si="0"/>
         <v>83</v>
@@ -4285,7 +4488,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="27">
+    <row r="85" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A85" s="2">
         <f t="shared" si="0"/>
         <v>84</v>
@@ -4309,7 +4512,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="27">
+    <row r="86" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A86" s="2">
         <f t="shared" si="0"/>
         <v>85</v>
@@ -4333,7 +4536,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="27">
+    <row r="87" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A87" s="2">
         <f t="shared" si="0"/>
         <v>86</v>
@@ -4357,7 +4560,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="27">
+    <row r="88" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A88" s="2">
         <f t="shared" si="0"/>
         <v>87</v>
@@ -4381,7 +4584,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="27">
+    <row r="89" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A89" s="2">
         <f t="shared" si="0"/>
         <v>88</v>
@@ -4405,7 +4608,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="27">
+    <row r="90" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A90" s="2">
         <f t="shared" si="0"/>
         <v>89</v>
@@ -4429,7 +4632,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="27">
+    <row r="91" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A91" s="2">
         <f t="shared" si="0"/>
         <v>90</v>
@@ -4453,7 +4656,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="27">
+    <row r="92" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A92" s="2">
         <f t="shared" si="0"/>
         <v>91</v>
@@ -4477,7 +4680,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="27">
+    <row r="93" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A93" s="2">
         <f t="shared" si="0"/>
         <v>92</v>
@@ -4501,7 +4704,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="27">
+    <row r="94" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A94" s="2">
         <f t="shared" si="0"/>
         <v>93</v>
@@ -4525,7 +4728,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="27">
+    <row r="95" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A95" s="2">
         <f t="shared" si="0"/>
         <v>94</v>
@@ -4549,7 +4752,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="27">
+    <row r="96" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A96" s="2">
         <f t="shared" si="0"/>
         <v>95</v>
@@ -4573,7 +4776,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="27">
+    <row r="97" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A97" s="2">
         <f t="shared" si="0"/>
         <v>96</v>
@@ -4597,7 +4800,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="27">
+    <row r="98" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A98" s="2">
         <f t="shared" si="0"/>
         <v>97</v>
@@ -4621,7 +4824,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="27">
+    <row r="99" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A99" s="2">
         <f t="shared" si="0"/>
         <v>98</v>
@@ -4645,7 +4848,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="27">
+    <row r="100" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A100" s="2">
         <f t="shared" si="0"/>
         <v>99</v>
@@ -4669,7 +4872,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="27">
+    <row r="101" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A101" s="2">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -4693,7 +4896,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="67.5">
+    <row r="102" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A102" s="2">
         <f t="shared" si="0"/>
         <v>101</v>
@@ -4717,7 +4920,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="67.5">
+    <row r="103" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A103" s="2">
         <f t="shared" si="0"/>
         <v>102</v>
@@ -4741,7 +4944,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="81">
+    <row r="104" spans="1:7" ht="81" x14ac:dyDescent="0.15">
       <c r="A104" s="2">
         <f t="shared" si="0"/>
         <v>103</v>
@@ -4765,7 +4968,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="81">
+    <row r="105" spans="1:7" ht="81" x14ac:dyDescent="0.15">
       <c r="A105" s="2">
         <f t="shared" si="0"/>
         <v>104</v>
@@ -4789,7 +4992,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="81">
+    <row r="106" spans="1:7" ht="81" x14ac:dyDescent="0.15">
       <c r="A106" s="2">
         <f t="shared" si="0"/>
         <v>105</v>
@@ -4813,7 +5016,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="81">
+    <row r="107" spans="1:7" ht="81" x14ac:dyDescent="0.15">
       <c r="A107" s="2">
         <f t="shared" si="0"/>
         <v>106</v>
@@ -4837,7 +5040,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="94.5">
+    <row r="108" spans="1:7" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A108" s="2">
         <f t="shared" si="0"/>
         <v>107</v>
@@ -4861,7 +5064,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="94.5">
+    <row r="109" spans="1:7" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A109" s="2">
         <f t="shared" si="0"/>
         <v>108</v>
@@ -4885,7 +5088,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="67.5">
+    <row r="110" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A110" s="2">
         <f t="shared" si="0"/>
         <v>109</v>
@@ -4909,7 +5112,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="67.5">
+    <row r="111" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A111" s="2">
         <f t="shared" si="0"/>
         <v>110</v>
@@ -4933,7 +5136,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="108">
+    <row r="112" spans="1:7" ht="108" x14ac:dyDescent="0.15">
       <c r="A112" s="2">
         <f t="shared" si="0"/>
         <v>111</v>
@@ -4957,7 +5160,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="108">
+    <row r="113" spans="1:7" ht="108" x14ac:dyDescent="0.15">
       <c r="A113" s="2">
         <f t="shared" si="0"/>
         <v>112</v>
@@ -4981,7 +5184,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="94.5">
+    <row r="114" spans="1:7" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A114" s="2">
         <f t="shared" si="0"/>
         <v>113</v>
@@ -5005,7 +5208,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="94.5">
+    <row r="115" spans="1:7" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A115" s="2">
         <f t="shared" si="0"/>
         <v>114</v>
@@ -5029,7 +5232,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="135">
+    <row r="116" spans="1:7" ht="135" x14ac:dyDescent="0.15">
       <c r="A116" s="2">
         <f t="shared" si="0"/>
         <v>115</v>
@@ -5053,7 +5256,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="135">
+    <row r="117" spans="1:7" ht="135" x14ac:dyDescent="0.15">
       <c r="A117" s="2">
         <f t="shared" si="0"/>
         <v>116</v>
@@ -5077,7 +5280,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="27">
+    <row r="118" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A118" s="2">
         <f t="shared" si="0"/>
         <v>117</v>
@@ -5095,13 +5298,13 @@
         <v>44</v>
       </c>
       <c r="F118" s="14" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G118" s="14" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" ht="27">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A119" s="2">
         <f t="shared" si="0"/>
         <v>118</v>
@@ -5122,10 +5325,10 @@
         <v>310</v>
       </c>
       <c r="G119" s="14" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" ht="27">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A120" s="2">
         <f t="shared" si="0"/>
         <v>119</v>
@@ -5143,13 +5346,13 @@
         <v>44</v>
       </c>
       <c r="F120" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G120" s="14" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" ht="27">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A121" s="2">
         <f t="shared" si="0"/>
         <v>120</v>
@@ -5167,15 +5370,15 @@
         <v>19</v>
       </c>
       <c r="F121" s="14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G121" s="14" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" ht="27">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A122" s="2">
-        <f t="shared" ref="A122:A124" si="2">ROW()-1</f>
+        <f t="shared" ref="A122:A138" si="2">ROW()-1</f>
         <v>121</v>
       </c>
       <c r="B122" s="7" t="s">
@@ -5191,13 +5394,13 @@
         <v>44</v>
       </c>
       <c r="F122" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="G122" s="14" t="s">
         <v>318</v>
       </c>
-      <c r="G122" s="14" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" ht="27">
+    </row>
+    <row r="123" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A123" s="2">
         <f t="shared" si="2"/>
         <v>122</v>
@@ -5215,23 +5418,359 @@
         <v>19</v>
       </c>
       <c r="F123" s="14" t="s">
+        <v>312</v>
+      </c>
+      <c r="G123" s="14" t="s">
         <v>313</v>
       </c>
-      <c r="G123" s="14" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7">
+    </row>
+    <row r="124" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A124" s="2">
         <f t="shared" si="2"/>
         <v>123</v>
       </c>
-      <c r="B124" s="15"/>
-      <c r="C124" s="15"/>
-      <c r="D124" s="2"/>
-      <c r="E124" s="2"/>
-      <c r="F124" s="14"/>
-      <c r="G124" s="14"/>
+      <c r="B124" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C124" s="16" t="s">
+        <v>320</v>
+      </c>
+      <c r="D124" s="17" t="s">
+        <v>321</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="F124" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="G124" s="14" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="A125" s="2">
+        <f t="shared" si="2"/>
+        <v>124</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C125" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="D125" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="F125" s="14" t="s">
+        <v>326</v>
+      </c>
+      <c r="G125" s="14" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="A126" s="2">
+        <f t="shared" si="2"/>
+        <v>125</v>
+      </c>
+      <c r="B126" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C126" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="D126" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="F126" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="G126" s="14" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="A127" s="2">
+        <f t="shared" si="2"/>
+        <v>126</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C127" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="D127" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="F127" s="14" t="s">
+        <v>333</v>
+      </c>
+      <c r="G127" s="14" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="A128" s="2">
+        <f t="shared" si="2"/>
+        <v>127</v>
+      </c>
+      <c r="B128" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C128" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="D128" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="F128" s="14" t="s">
+        <v>336</v>
+      </c>
+      <c r="G128" s="14" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="A129" s="2">
+        <f t="shared" si="2"/>
+        <v>128</v>
+      </c>
+      <c r="B129" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C129" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="D129" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="F129" s="14" t="s">
+        <v>337</v>
+      </c>
+      <c r="G129" s="14" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="A130" s="2">
+        <f t="shared" si="2"/>
+        <v>129</v>
+      </c>
+      <c r="B130" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="C130" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="D130" s="17" t="s">
+        <v>340</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="F130" s="14" t="s">
+        <v>341</v>
+      </c>
+      <c r="G130" s="14" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="A131" s="2">
+        <f t="shared" si="2"/>
+        <v>130</v>
+      </c>
+      <c r="B131" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="C131" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="D131" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="F131" s="14" t="s">
+        <v>342</v>
+      </c>
+      <c r="G131" s="14" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="A132" s="2">
+        <f t="shared" si="2"/>
+        <v>131</v>
+      </c>
+      <c r="B132" s="16" t="s">
+        <v>348</v>
+      </c>
+      <c r="C132" s="16" t="s">
+        <v>320</v>
+      </c>
+      <c r="D132" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="E132" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F132" s="14" t="s">
+        <v>349</v>
+      </c>
+      <c r="G132" s="14" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="A133" s="2">
+        <f t="shared" si="2"/>
+        <v>132</v>
+      </c>
+      <c r="B133" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="C133" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="D133" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F133" s="14" t="s">
+        <v>350</v>
+      </c>
+      <c r="G133" s="14" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="A134" s="2">
+        <f t="shared" si="2"/>
+        <v>133</v>
+      </c>
+      <c r="B134" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="C134" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="D134" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F134" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="G134" s="14" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="A135" s="2">
+        <f t="shared" si="2"/>
+        <v>134</v>
+      </c>
+      <c r="B135" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="C135" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="D135" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="E135" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F135" s="14" t="s">
+        <v>338</v>
+      </c>
+      <c r="G135" s="14" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="A136" s="2">
+        <f t="shared" si="2"/>
+        <v>135</v>
+      </c>
+      <c r="B136" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="C136" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="D136" s="17" t="s">
+        <v>340</v>
+      </c>
+      <c r="E136" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F136" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="G136" s="14" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="A137" s="2">
+        <f t="shared" si="2"/>
+        <v>136</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="C137" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="D137" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F137" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="G137" s="14" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A138" s="2">
+        <f t="shared" si="2"/>
+        <v>137</v>
+      </c>
+      <c r="B138" s="15"/>
+      <c r="C138" s="15"/>
+      <c r="D138" s="2"/>
+      <c r="E138" s="2"/>
+      <c r="F138" s="14"/>
+      <c r="G138" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>